<commit_message>
Final de refactor y horas
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D25FD3-122C-4027-A783-574C00C6B617}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5B0903-C4BA-477E-B020-4ACACBFE841C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Roberto</t>
   </si>
@@ -163,30 +163,59 @@
     <t>No entregado</t>
   </si>
   <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación login angular</t>
+  </si>
+  <si>
     <t>- Implementacion metodo put en back
-- Metodo comprobación correo OK</t>
+- Metodo comprobación correo OK
+- Implementación menu angular</t>
   </si>
   <si>
     <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Roberto =&gt; Login back y front
+- Metodo comprobación correo OK
+- Implementación menu angular</t>
+  </si>
+  <si>
+    <t>- Gestion de horas y tareas
+- Conexión front-back
+- Refactor y documentacion
+- Implementación registro angular</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Roberto =&gt; Login back y front
 Irantzu + Carlos =&gt; Menu
 Sergio =&gt; Registro</t>
-  </si>
-  <si>
-    <t>- Gestion de horas y tareas
-- Conexión front-back
-- Refactor y documentacion</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,8 +268,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +320,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -622,6 +665,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -640,65 +716,32 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,13 +765,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>714375</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>457201</xdr:colOff>
+      <xdr:colOff>714376</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -745,8 +788,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5314950" y="0"/>
-          <a:ext cx="1" cy="4629150"/>
+          <a:off x="5743575" y="0"/>
+          <a:ext cx="1" cy="5048250"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1077,7 +1120,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,57 +1137,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="17" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="22"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="33"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1194,7 +1237,7 @@
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -1214,7 +1257,7 @@
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -1234,7 +1277,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
@@ -1268,239 +1311,244 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="23" t="s">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="23" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="23" t="s">
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
+      <c r="B10" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1508,13 +1556,9 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Version de registro conectada a back y base de datos
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5B0903-C4BA-477E-B020-4ACACBFE841C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F87F4F4-A495-4DB0-84DD-BD342AB3A049}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
@@ -178,12 +178,6 @@
 - Implementación menu angular</t>
   </si>
   <si>
-    <t>- Gestion de horas y tareas
-- Conexión front-back
-- Refactor y documentacion
-- Implementación registro angular</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -209,6 +203,12 @@
 Irantzu + Carlos =&gt; Menu
 Sergio =&gt; Registro</t>
     </r>
+  </si>
+  <si>
+    <t>- Gestion de horas y tareas
+- Conexión front-back registro
+- Refactor y documentacion
+- Implementación registro angular</t>
   </si>
 </sst>
 </file>
@@ -665,6 +665,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -692,29 +716,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
@@ -739,9 +742,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,7 +1120,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,57 +1137,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="28" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="28" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="29"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="28" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="29"/>
-      <c r="N1" s="30"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="33"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="31"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="33"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1297,7 +1297,7 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1311,244 +1311,239 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="26" t="s">
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="26" t="s">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
+      <c r="B10" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="36"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="39"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1556,6 +1551,11 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Intento de hosteo BBDD azure
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952905FE-9865-4804-97D9-92DE19F74667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4A9BF6-F02A-40D1-9141-104B810C159D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Funciones" sheetId="1" r:id="rId1"/>
+    <sheet name="Protocolo dayly" sheetId="2" r:id="rId2"/>
+    <sheet name="Problemas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Roberto</t>
   </si>
@@ -163,21 +165,6 @@
     <t>No entregado</t>
   </si>
   <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación login angular</t>
-  </si>
-  <si>
-    <t>- Implementacion metodo put en back
-- Metodo comprobación correo OK
-- Implementación menu angular</t>
-  </si>
-  <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación menu angular</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -205,10 +192,52 @@
     </r>
   </si>
   <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación login angular
+- Delete Usuarios back
+- Troubleshooting angular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Troubleshooting angular
+- Graficos: mapa
+</t>
+  </si>
+  <si>
+    <t>33
+ (aprox)</t>
+  </si>
+  <si>
+    <t>2. Qué problemas encontrasteis?</t>
+  </si>
+  <si>
+    <t>1. Qué hicisteis ayer?</t>
+  </si>
+  <si>
+    <t>- Implementacion metodo put en back
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Graficos: otros
+- Crear menu front</t>
+  </si>
+  <si>
+    <t>Paginacion, problemas a la hora de meter el grafico.</t>
+  </si>
+  <si>
+    <t>3. Qué hacemos hoy?</t>
+  </si>
+  <si>
+    <t>Cuello de botella BBDD y datos para hacer graficos</t>
+  </si>
+  <si>
     <t>- Gestion de horas y tareas
 - Conexión front-back registro
 - Refactor y documentacion
-- Implementación registro angular</t>
+- Implementación registro angular
+- BBDD azure</t>
   </si>
 </sst>
 </file>
@@ -617,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -665,6 +694,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -719,29 +772,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1120,7 +1152,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,57 +1169,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="37" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="37" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="37" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="38"/>
-      <c r="N1" s="39"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1237,9 +1269,11 @@
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>26</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -1259,7 +1293,9 @@
       <c r="D6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10">
+        <v>33</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -1277,9 +1313,11 @@
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="E7" s="10">
+        <v>33</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -1297,9 +1335,11 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="E8" s="13">
+        <v>33</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -1311,244 +1351,239 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="35" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="35" t="s">
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="35" t="s">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
+      <c r="B10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="20"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20"/>
-      <c r="N13" s="20"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="20"/>
-      <c r="N14" s="20"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="19"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="19"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1556,9 +1591,72 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527D0FE6-87E0-4186-A41F-3E960C5F4290}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC113B12-C74D-416E-884F-DBDB84D406B9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se elimina routing deprecated
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4A9BF6-F02A-40D1-9141-104B810C159D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC314B7D-4A41-4C35-99C2-2F24310B3C5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Roberto</t>
   </si>
@@ -165,15 +165,23 @@
     <t>No entregado</t>
   </si>
   <si>
+    <t>33
+ (aprox)</t>
+  </si>
+  <si>
+    <t>2. Qué problemas encontrasteis?</t>
+  </si>
+  <si>
+    <t>1. Qué hicisteis ayer?</t>
+  </si>
+  <si>
+    <t>Paginacion, problemas a la hora de meter el grafico.</t>
+  </si>
+  <si>
+    <t>3. Qué hacemos hoy?</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
 </t>
     </r>
@@ -187,7 +195,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>Roberto =&gt; Login back y front
-Irantzu + Carlos =&gt; Menu
+Irantzu + Carlos + Roberto =&gt; Menu
 Sergio =&gt; Registro</t>
     </r>
   </si>
@@ -196,48 +204,41 @@
 - Metodo comprobación correo OK
 - Implementación login angular
 - Delete Usuarios back
-- Troubleshooting angular</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- Diseño funcionalidades menu
+- Troubleshooting angular
+- Outliers del menu
+- Investigación gráficas angular</t>
+  </si>
+  <si>
+    <t>- Implementacion metodo put en back
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Graficos menu: otros + mapa + spaguetti
+- Crear menu front</t>
+  </si>
+  <si>
+    <t>Grafico de mapa, no conseguimos que funcione.</t>
+  </si>
+  <si>
+    <t>Cuello de botella BBDD y datos para hacer graficos.</t>
+  </si>
+  <si>
+    <t>- Diseño funcionalidades menu
 - Metodo comprobación correo OK
 - Implementación menu angular
 - Troubleshooting angular
 - Graficos: mapa
-</t>
-  </si>
-  <si>
-    <t>33
- (aprox)</t>
-  </si>
-  <si>
-    <t>2. Qué problemas encontrasteis?</t>
-  </si>
-  <si>
-    <t>1. Qué hicisteis ayer?</t>
-  </si>
-  <si>
-    <t>- Implementacion metodo put en back
-- Metodo comprobación correo OK
-- Implementación menu angular
-- Graficos: otros
-- Crear menu front</t>
-  </si>
-  <si>
-    <t>Paginacion, problemas a la hora de meter el grafico.</t>
-  </si>
-  <si>
-    <t>3. Qué hacemos hoy?</t>
-  </si>
-  <si>
-    <t>Cuello de botella BBDD y datos para hacer graficos</t>
+- Dayly y Scrum^2
+- Codigo predicción</t>
   </si>
   <si>
     <t>- Gestion de horas y tareas
 - Conexión front-back registro
 - Refactor y documentacion
 - Implementación registro angular
-- BBDD azure</t>
+- BBDD azure
+- Creación servicio front azure
+- Workflows github
+- Configuración routing</t>
   </si>
 </sst>
 </file>
@@ -694,6 +695,69 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -711,69 +775,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1152,7 +1153,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,57 +1170,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="17" t="s">
+      <c r="J1" s="39"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="22"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1262,17 +1263,17 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>26</v>
+        <v>29</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1284,14 +1285,14 @@
       <c r="M5" s="10"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="16" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E6" s="10">
         <v>33</v>
@@ -1313,7 +1314,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="10">
         <v>33</v>
@@ -1328,14 +1329,14 @@
       <c r="M7" s="10"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E8" s="13">
         <v>33</v>
@@ -1351,239 +1352,244 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="23" t="s">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="23" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="23" t="s">
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
+      <c r="B10" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="20"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="20"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="20"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1591,11 +1597,6 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1608,7 +1609,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,17 +1619,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1638,22 +1639,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC113B12-C74D-416E-884F-DBDB84D406B9}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solucion routing tras merge
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC314B7D-4A41-4C35-99C2-2F24310B3C5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E325F397-E991-42E4-8B09-717BFFBE9607}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Roberto</t>
   </si>
@@ -165,10 +165,6 @@
     <t>No entregado</t>
   </si>
   <si>
-    <t>33
- (aprox)</t>
-  </si>
-  <si>
     <t>2. Qué problemas encontrasteis?</t>
   </si>
   <si>
@@ -179,6 +175,48 @@
   </si>
   <si>
     <t>3. Qué hacemos hoy?</t>
+  </si>
+  <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación login angular
+- Delete Usuarios back
+- Troubleshooting angular
+- Outliers del menu
+- Investigación gráficas angular</t>
+  </si>
+  <si>
+    <t>- Implementacion metodo put en back
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Graficos menu: otros + mapa + spaguetti
+- Crear menu front</t>
+  </si>
+  <si>
+    <t>Grafico de mapa, no conseguimos que funcione.</t>
+  </si>
+  <si>
+    <t>Cuello de botella BBDD y datos para hacer graficos.</t>
+  </si>
+  <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Troubleshooting angular
+- Graficos: mapa
+- Dayly y Scrum^2
+- Codigo predicción</t>
+  </si>
+  <si>
+    <t>- Gestion de horas y tareas
+- Conexión front-back registro
+- Refactor y documentacion
+- Implementación registro angular
+- BBDD azure
+- Creación servicio front azure
+- Workflows github
+- Configuración routing
+- Gestión rama producción</t>
   </si>
   <si>
     <r>
@@ -195,50 +233,31 @@
         <scheme val="minor"/>
       </rPr>
       <t>Roberto =&gt; Login back y front
-Irantzu + Carlos + Roberto =&gt; Menu
+Irantzu + Carlos + Roberto =&gt; Menu + Funcionalidades + Datos
 Sergio =&gt; Registro</t>
     </r>
-  </si>
-  <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación login angular
-- Delete Usuarios back
-- Troubleshooting angular
-- Outliers del menu
-- Investigación gráficas angular</t>
-  </si>
-  <si>
-    <t>- Implementacion metodo put en back
-- Metodo comprobación correo OK
-- Implementación menu angular
-- Graficos menu: otros + mapa + spaguetti
-- Crear menu front</t>
-  </si>
-  <si>
-    <t>Grafico de mapa, no conseguimos que funcione.</t>
-  </si>
-  <si>
-    <t>Cuello de botella BBDD y datos para hacer graficos.</t>
-  </si>
-  <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación menu angular
-- Troubleshooting angular
-- Graficos: mapa
-- Dayly y Scrum^2
-- Codigo predicción</t>
-  </si>
-  <si>
-    <t>- Gestion de horas y tareas
-- Conexión front-back registro
-- Refactor y documentacion
-- Implementación registro angular
-- BBDD azure
-- Creación servicio front azure
-- Workflows github
-- Configuración routing</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFFFF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>+ DevOps</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -647,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -695,8 +714,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,28 +792,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1153,7 +1178,7 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,57 +1195,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="38" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="38" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="39"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="38" t="s">
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="40"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="43"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="41"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1270,10 +1295,10 @@
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="E5" s="43">
+        <v>33</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1292,9 +1317,9 @@
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10">
+        <v>31</v>
+      </c>
+      <c r="E6" s="44">
         <v>33</v>
       </c>
       <c r="F6" s="10"/>
@@ -1314,9 +1339,9 @@
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="10">
+        <v>28</v>
+      </c>
+      <c r="E7" s="44">
         <v>33</v>
       </c>
       <c r="F7" s="10"/>
@@ -1329,16 +1354,16 @@
       <c r="M7" s="10"/>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="1:14" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="13">
+        <v>32</v>
+      </c>
+      <c r="E8" s="45">
         <v>33</v>
       </c>
       <c r="F8" s="13"/>
@@ -1352,244 +1377,239 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="36" t="s">
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="36" t="s">
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="36" t="s">
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="B10" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="35"/>
+      <c r="D10" s="35"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="20"/>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="20"/>
-      <c r="M12" s="21"/>
-      <c r="N12" s="21"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="20"/>
-      <c r="M13" s="21"/>
-      <c r="N13" s="21"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="20"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="30"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="21"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="30"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="30"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="21"/>
-      <c r="N20" s="21"/>
+      <c r="B20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="30"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
+      <c r="K22" s="30"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1597,6 +1617,11 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1619,17 +1644,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1649,17 +1674,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se configuran variables de entorno
</commit_message>
<xml_diff>
--- a/docs/Horas proyecto estadistica.xlsx
+++ b/docs/Horas proyecto estadistica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Trabajo_final\AppClientesEstadistica\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E325F397-E991-42E4-8B09-717BFFBE9607}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A2BEBB-4897-4A12-840B-D9F9F5A70DBC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12315" windowHeight="7980" xr2:uid="{75DE17B3-81B2-44DB-AF0F-61090BDD4A63}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Roberto</t>
   </si>
@@ -177,35 +177,10 @@
     <t>3. Qué hacemos hoy?</t>
   </si>
   <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación login angular
-- Delete Usuarios back
-- Troubleshooting angular
-- Outliers del menu
-- Investigación gráficas angular</t>
-  </si>
-  <si>
-    <t>- Implementacion metodo put en back
-- Metodo comprobación correo OK
-- Implementación menu angular
-- Graficos menu: otros + mapa + spaguetti
-- Crear menu front</t>
-  </si>
-  <si>
     <t>Grafico de mapa, no conseguimos que funcione.</t>
   </si>
   <si>
     <t>Cuello de botella BBDD y datos para hacer graficos.</t>
-  </si>
-  <si>
-    <t>- Diseño funcionalidades menu
-- Metodo comprobación correo OK
-- Implementación menu angular
-- Troubleshooting angular
-- Graficos: mapa
-- Dayly y Scrum^2
-- Codigo predicción</t>
   </si>
   <si>
     <t>- Gestion de horas y tareas
@@ -258,6 +233,52 @@
       </rPr>
       <t>+ DevOps</t>
     </r>
+  </si>
+  <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación login angular
+- Delete Usuarios back
+- Troubleshooting angular
+- Outliers del menu
+- Investigación gráficas angular
+- Bogus (creacion datos)</t>
+  </si>
+  <si>
+    <t>- Bogus
+- Implementar Bogus a front
+- Arreglar tostadora (ordenador)</t>
+  </si>
+  <si>
+    <t>- Diseño funcionalidades menu
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Troubleshooting angular
+- Graficos: mapa
+- Dayly y Scrum^2
+- Codigo predicción
+- Conectar python a C#</t>
+  </si>
+  <si>
+    <t>- Conectar python a C#</t>
+  </si>
+  <si>
+    <t>- Implementacion metodo put en back
+- Metodo comprobación correo OK
+- Implementación menu angular
+- Graficos menu: otros + mapa + spaguetti
+- Crear menu front
+- Graficos
+- Tablas</t>
+  </si>
+  <si>
+    <t>- Selectores dropdown para elegir moneda
+- Clusters conectar datos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Hosteo en Azure
+- Variables de entorno
+</t>
   </si>
 </sst>
 </file>
@@ -666,7 +687,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -714,6 +735,75 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -732,74 +822,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1177,8 +1201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{609C8817-5D91-4583-A706-CC11F2A98614}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,57 +1219,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="17" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="17" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="17" t="s">
+      <c r="J1" s="41"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="42"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="22"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="45"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="44"/>
+      <c r="N3" s="45"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -1288,19 +1312,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10"/>
       <c r="D5" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="43">
+        <v>31</v>
+      </c>
+      <c r="E5" s="17">
         <v>33</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="16" t="s">
+        <v>32</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
@@ -1310,19 +1336,21 @@
       <c r="M5" s="10"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="1:14" ht="84.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="96.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="10"/>
       <c r="D6" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="44">
         <v>33</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="E6" s="18">
+        <v>33</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>34</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -1332,19 +1360,21 @@
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="1:14" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="10"/>
       <c r="D7" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="44">
+        <v>35</v>
+      </c>
+      <c r="E7" s="18">
         <v>33</v>
       </c>
-      <c r="F7" s="10"/>
+      <c r="F7" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -1361,12 +1391,14 @@
       <c r="B8" s="12"/>
       <c r="C8" s="13"/>
       <c r="D8" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="45">
+        <v>29</v>
+      </c>
+      <c r="E8" s="19">
         <v>33</v>
       </c>
-      <c r="F8" s="13"/>
+      <c r="F8" s="15" t="s">
+        <v>37</v>
+      </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
@@ -1377,239 +1409,244 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="23" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="23" t="s">
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="23" t="s">
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
+      <c r="M9" s="39"/>
+      <c r="N9" s="39"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
+      <c r="B10" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="37"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="37"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="37"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="37"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="37"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="37"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="37"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="22"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="37"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
     </row>
     <row r="22" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="L1:N3"/>
+    <mergeCell ref="I1:K3"/>
+    <mergeCell ref="F1:H3"/>
+    <mergeCell ref="L9:N9"/>
     <mergeCell ref="L10:N22"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E22"/>
@@ -1617,11 +1654,6 @@
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="I10:K22"/>
-    <mergeCell ref="B1:E3"/>
-    <mergeCell ref="L1:N3"/>
-    <mergeCell ref="I1:K3"/>
-    <mergeCell ref="F1:H3"/>
-    <mergeCell ref="L9:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1679,12 +1711,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>